<commit_message>
added one mroe dataset on agriculture
</commit_message>
<xml_diff>
--- a/data/NRV-wells-floyd-county-2011.xlsx
+++ b/data/NRV-wells-floyd-county-2011.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Floyd-County/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Floyd-County/DSPG_Floyd/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26855271-6A2D-C444-B12C-7F3F67FF1ADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D64054-AEA9-FB4C-8F1D-985FAB9DAAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{FC4880B3-BD6B-1D4F-B799-BC93BF8A556F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t xml:space="preserve">Name and ID </t>
   </si>
@@ -57,9 +57,6 @@
     <t xml:space="preserve">Well Depth (ft) </t>
   </si>
   <si>
-    <t>NI</t>
-  </si>
-  <si>
     <t xml:space="preserve">Casing Depth (ft) </t>
   </si>
   <si>
@@ -103,114 +100,6 @@
   </si>
   <si>
     <t xml:space="preserve">System Permitted Capacity: </t>
-  </si>
-  <si>
-    <t>Large Self-supplied Nonagricultural Users</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Great Oaks Country Club </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pond </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average Daily Withdrawal (MGD) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum Daily Withdrawal (MGD) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limitations on Withdrawal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source </t>
-  </si>
-  <si>
-    <t>Number of farms (irrigated)</t>
-  </si>
-  <si>
-    <t>Acres irrigated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average size of irrigated farms (acres) </t>
-  </si>
-  <si>
-    <t>Acres in farming</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of farms  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average farm size (acres) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cattle &amp; Calves </t>
-  </si>
-  <si>
-    <t>Farms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hogs &amp; Pigs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poultry </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Horses &amp; Ponies </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sheep &amp; Lambs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goats </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of animals </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average animals per farm </t>
-  </si>
-  <si>
-    <t>Number of animals</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Average animals per farm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bees </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Average animals per farm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of colonies </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average colonies per farm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Livestock </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimates of Small Self-supplied Nonagricultural Users </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Population </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Population Served by CWS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Est. Population Served by Wells </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent Served by Wells </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Est. Residences on Wells </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Est. Businesses on Wells </t>
   </si>
 </sst>
 </file>
@@ -594,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F760C6E7-4E91-9649-B45B-D5CF9D19ACA9}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="117" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -630,7 +519,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -670,7 +559,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>52</v>
@@ -690,7 +579,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -710,406 +599,174 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2.4400000000000002E-2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16">
-        <v>128872</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19">
-        <v>5856</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25">
-        <v>38353</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B29">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B33">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37">
-        <v>1169</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B41">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B44">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
-      <c r="A45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
-      <c r="A46" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48">
-        <v>15</v>
-      </c>
+      <c r="A15" s="1"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="1"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="1"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50">
-        <v>2</v>
-      </c>
+      <c r="A49" s="1"/>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55">
-        <v>13874</v>
-      </c>
+      <c r="A54" s="4"/>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56">
-        <v>2347</v>
-      </c>
+      <c r="A56" s="2"/>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57">
-        <v>11527</v>
-      </c>
+      <c r="A57" s="2"/>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="5">
-        <v>0.83</v>
-      </c>
+      <c r="A58" s="2"/>
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59">
-        <v>4823</v>
-      </c>
+      <c r="A59" s="2"/>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B60">
-        <v>23</v>
-      </c>
+      <c r="A60" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cleaned up graphs for precipation and temperature. Added a group of Floyd with points
</commit_message>
<xml_diff>
--- a/data/NRV-wells-floyd-county-2011.xlsx
+++ b/data/NRV-wells-floyd-county-2011.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Floyd-County/DSPG_Floyd/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D64054-AEA9-FB4C-8F1D-985FAB9DAAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A44027-53ED-6547-A5EE-960D75517D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{FC4880B3-BD6B-1D4F-B799-BC93BF8A556F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t xml:space="preserve">Name and ID </t>
   </si>
@@ -63,24 +63,6 @@
     <t xml:space="preserve">Well Diameter (ft) </t>
   </si>
   <si>
-    <t xml:space="preserve">Average Daily Withdrawal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.03 MGD (29,000 gpd) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.03 MGD (27,800 gpd) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.03 MGD (25,500 gpd) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.03 MGD (25,700 gpd) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.04 MGD (40,000 gpd) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Design Capacity- Max Daily </t>
   </si>
   <si>
@@ -100,6 +82,12 @@
   </si>
   <si>
     <t xml:space="preserve">System Permitted Capacity: </t>
+  </si>
+  <si>
+    <t>Average Daily Withdrawal (MGD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Daily Withdrawal (gpd) </t>
   </si>
 </sst>
 </file>
@@ -160,13 +148,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F760C6E7-4E91-9649-B45B-D5CF9D19ACA9}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:F61"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -519,7 +508,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -599,62 +588,102 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="6">
+        <v>29000</v>
+      </c>
+      <c r="C7" s="6">
+        <v>27800</v>
+      </c>
+      <c r="D7" s="6">
+        <v>25500</v>
+      </c>
+      <c r="E7" s="6">
+        <v>25700</v>
+      </c>
+      <c r="F7" s="6">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="25" customHeight="1">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B8" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="25" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6">
+        <v>68400</v>
+      </c>
+      <c r="C9" s="6">
+        <v>43200</v>
+      </c>
+      <c r="D9" s="6">
+        <v>36000</v>
+      </c>
+      <c r="E9" s="6">
+        <v>36000</v>
+      </c>
+      <c r="F9" s="6">
+        <v>115200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="25" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6">

</xml_diff>